<commit_message>
Atualização automática de CRISSIUMAL.xlsx
</commit_message>
<xml_diff>
--- a/CRISSIUMAL.xlsx
+++ b/CRISSIUMAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C2479CB-49E8-4A71-8EDE-F9DEEDAFE8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{26E5FF0C-DD91-4C64-BDA7-2D3B9A75AA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,20 +21,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="5" r:id="rId6"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1074,7 +1061,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1134,36 +1121,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1202,14 +1165,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1255,7 +1213,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{E8E1EF58-A776-4B3C-90AB-F2BC3680D509}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{04C33F05-3D2C-4D94-9285-573355ED1F0E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1285,10 +1243,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B1B0A2F-C056-44CC-A533-8BD57D06C917}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{844C8EF8-2B7A-4B8C-AA6F-A94EB395DD2E}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1326,7 +1284,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2D88106-1DB7-428B-AE7F-67283FE3636B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D78980CF-09BA-45C1-AB82-06DD8700EB2F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1389,7 +1347,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08A27981-2111-44FA-A35B-AD2700D5F44D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{587B298F-2E9F-49C3-A86F-D130B1F12504}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1408,7 +1366,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8419097-6846-66E2-5771-8AA27FFE8181}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2864FA95-2B67-668B-E228-7E8B656AB99F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1457,7 +1415,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67974E5A-F5E2-C414-B8A5-06D60DD4E7D0}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EB7983A-BFE8-DD33-500B-013CFDF19719}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1476,7 +1434,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75B5718E-1F88-65F0-BE4C-CBC4E1539E1A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C01C4E9B-9367-0DF8-8630-434DCCB4CB96}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1507,7 +1465,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD99A13F-CFB0-DBBD-7406-D9AABF830867}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB06BBEB-AA94-8287-2123-33765A004655}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1538,7 +1496,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8AEA9E6-81AD-14B1-E072-3BDF0AF1BCA4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1C5E04D-097A-D6CA-8437-316744901CBD}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1581,7 +1539,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D5AB6EC-6BCF-459E-A267-87357CB7DE90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9C995B6-F393-42AF-A484-D05DC8E65AB4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1619,7 +1577,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36126687-9FDF-49F7-BC2C-794A37083E5C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BC23A73-C6D8-4E24-9D8A-A9D49CDEF9AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1662,7 +1620,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8B81735-C511-4CD0-BDB0-CF210850C76F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4A9FF44-F22D-4495-B55F-8353C366A2F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1975,7 +1933,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E30157-BDDB-4162-91CA-FA50B9994122}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8367AEC5-CA95-4AF3-BE02-A30EE464F303}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1987,98 +1945,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="37"/>
-    <col min="6" max="6" width="2" style="37" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="37" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="37"/>
+    <col min="1" max="5" width="12.5703125" style="34"/>
+    <col min="6" max="6" width="2" style="34" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="34" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="36"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="36"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="36"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="36"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="36"/>
+      <c r="F5" s="33"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="36"/>
+      <c r="F6" s="33"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="36"/>
+      <c r="F7" s="33"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="36"/>
+      <c r="F8" s="33"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="36"/>
+      <c r="F9" s="33"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="36"/>
+      <c r="F10" s="33"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="36"/>
+      <c r="F11" s="33"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="36"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="36"/>
+      <c r="F13" s="33"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="36"/>
+      <c r="F14" s="33"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="36"/>
+      <c r="F15" s="33"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="36"/>
+      <c r="F16" s="33"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="36"/>
+      <c r="F17" s="33"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="36"/>
+      <c r="F18" s="33"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="36"/>
+      <c r="F19" s="33"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="36"/>
+      <c r="F20" s="33"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="36"/>
+      <c r="F21" s="33"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="36"/>
+      <c r="F22" s="33"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="36"/>
+      <c r="F23" s="33"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="36"/>
+      <c r="F24" s="33"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="36"/>
+      <c r="F25" s="33"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="36"/>
+      <c r="F26" s="33"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="36"/>
+      <c r="F27" s="33"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="36"/>
+      <c r="F28" s="33"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="36"/>
+      <c r="F29" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5342,19 +5300,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>272</v>
       </c>
     </row>
@@ -5377,46 +5335,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>276</v>
       </c>
     </row>
@@ -5441,54 +5399,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>280</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="21" t="s">
         <v>284</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="22" t="s">
         <v>285</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="20" t="s">
         <v>290</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="20" t="s">
         <v>291</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="20" t="s">
         <v>293</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="20" t="s">
         <v>294</v>
       </c>
     </row>
@@ -5499,43 +5458,43 @@
       <c r="B2" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="23">
         <v>45717</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="24">
         <v>3369</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="24" t="s">
         <v>296</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="25">
         <v>3941</v>
       </c>
-      <c r="G2" s="28">
+      <c r="G2" s="25">
         <v>345</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="M2" s="30" t="s">
+      <c r="M2" s="27" t="s">
         <v>298</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="O2" s="30" t="s">
+      <c r="O2" s="27" t="s">
         <v>298</v>
       </c>
     </row>
@@ -5566,25 +5525,24 @@
       <c r="B1" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="28" t="s">
         <v>301</v>
       </c>
-      <c r="E1" s="32">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="29">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2" s="32">
         <v>25</v>
       </c>
-      <c r="F1" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>302</v>
-      </c>
-      <c r="B2" s="35">
-        <v>25</v>
-      </c>
-      <c r="C2" s="33">
+      <c r="C2" s="30">
         <v>1.653220473482344E-3</v>
       </c>
     </row>

</xml_diff>